<commit_message>
finished download for invoice
</commit_message>
<xml_diff>
--- a/counts/static/counts/CountTemplate.xlsx
+++ b/counts/static/counts/CountTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvickers\Desktop\Inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvickers\Desktop\simpledarius\secundarius\counts\static\counts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF45823-A6E0-4E83-8621-0B120CDA69D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306D5921-3ECF-4B83-86EC-FEEF8A195606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-15360" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t>Item Code</t>
   </si>
@@ -472,6 +472,18 @@
   </si>
   <si>
     <t>TO INVOICE</t>
+  </si>
+  <si>
+    <t>Yogurt - Plain 24 oz.</t>
+  </si>
+  <si>
+    <t>MG1401</t>
+  </si>
+  <si>
+    <t>MG1409</t>
+  </si>
+  <si>
+    <t>Flavorpac Broccoli Cuts</t>
   </si>
 </sst>
 </file>
@@ -481,7 +493,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#############"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -516,6 +528,13 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="ARIAL"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -816,7 +835,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -971,6 +990,23 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1354,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8360C6-FEA5-4AEC-A5A3-073BC3CDB78F}">
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1600,13 +1636,13 @@
       <c r="M11" s="27"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="41">
+      <c r="A12" s="67" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="68" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="69">
         <v>12</v>
       </c>
       <c r="D12" s="45"/>
@@ -1619,14 +1655,14 @@
       <c r="M12" s="27"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="29">
-        <v>30</v>
+      <c r="A13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="41">
+        <v>12</v>
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="47"/>
@@ -1639,13 +1675,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="29">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="47"/>
@@ -1658,10 +1694,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="29">
         <v>12</v>
@@ -1677,10 +1713,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="29">
         <v>12</v>
@@ -1696,13 +1732,13 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="29">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="47"/>
@@ -1714,14 +1750,14 @@
       <c r="M17" s="27"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="30">
-        <v>9</v>
+      <c r="A18" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="64">
+        <v>12</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="47"/>
@@ -1733,14 +1769,14 @@
       <c r="M18" s="27"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="29">
-        <v>12</v>
+      <c r="A19" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="66">
+        <v>9</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="47"/>
@@ -1752,14 +1788,14 @@
       <c r="M19" s="27"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="31">
-        <v>24</v>
+      <c r="A20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="30">
+        <v>9</v>
       </c>
       <c r="D20" s="45"/>
       <c r="E20" s="47"/>
@@ -1771,14 +1807,14 @@
       <c r="M20" s="27"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="31">
-        <v>24</v>
+      <c r="A21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="29">
+        <v>12</v>
       </c>
       <c r="D21" s="45"/>
       <c r="E21" s="47"/>
@@ -1791,10 +1827,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C22" s="31">
         <v>24</v>
@@ -1810,10 +1846,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="C23" s="31">
         <v>24</v>
@@ -1829,10 +1865,10 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24" s="31">
         <v>24</v>
@@ -1848,10 +1884,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C25" s="31">
         <v>24</v>
@@ -1866,14 +1902,14 @@
       <c r="M25" s="27"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="30">
-        <v>48</v>
+      <c r="A26" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="31">
+        <v>24</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="47"/>
@@ -1885,13 +1921,13 @@
       <c r="M26" s="27"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="30">
+      <c r="A27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="31">
         <v>24</v>
       </c>
       <c r="D27" s="45"/>
@@ -1905,13 +1941,13 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C28" s="30">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="47"/>
@@ -1923,13 +1959,13 @@
       <c r="M28" s="27"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="32">
+      <c r="A29" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="30">
         <v>24</v>
       </c>
       <c r="D29" s="45"/>
@@ -1942,13 +1978,13 @@
       <c r="M29" s="27"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="32">
+      <c r="A30" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="30">
         <v>24</v>
       </c>
       <c r="D30" s="45"/>
@@ -1962,10 +1998,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="C31" s="32">
         <v>24</v>
@@ -1979,15 +2015,15 @@
       <c r="L31" s="27"/>
       <c r="M31" s="27"/>
     </row>
-    <row r="32" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="33">
-        <v>10</v>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="32">
+        <v>24</v>
       </c>
       <c r="D32" s="45"/>
       <c r="E32" s="47"/>
@@ -1998,15 +2034,15 @@
       <c r="L32" s="27"/>
       <c r="M32" s="27"/>
     </row>
-    <row r="33" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="33">
-        <v>10</v>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="32">
+        <v>24</v>
       </c>
       <c r="D33" s="45"/>
       <c r="E33" s="47"/>
@@ -2017,15 +2053,15 @@
       <c r="L33" s="27"/>
       <c r="M33" s="27"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="34">
-        <v>36</v>
+    <row r="34" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="33">
+        <v>10</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="47"/>
@@ -2037,14 +2073,14 @@
       <c r="M34" s="27"/>
     </row>
     <row r="35" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="17" t="s">
-        <v>68</v>
+      <c r="A35" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C35" s="33">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="47"/>
@@ -2055,15 +2091,15 @@
       <c r="L35" s="27"/>
       <c r="M35" s="27"/>
     </row>
-    <row r="36" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="35">
-        <v>12</v>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="34">
+        <v>36</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="47"/>
@@ -2075,14 +2111,14 @@
       <c r="M36" s="27"/>
     </row>
     <row r="37" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="36">
-        <v>6</v>
+      <c r="A37" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="33">
+        <v>12</v>
       </c>
       <c r="D37" s="45"/>
       <c r="E37" s="47"/>
@@ -2093,15 +2129,15 @@
       <c r="L37" s="27"/>
       <c r="M37" s="27"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="37">
-        <v>30</v>
+    <row r="38" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="35">
+        <v>12</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="47"/>
@@ -2114,13 +2150,13 @@
     </row>
     <row r="39" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C39" s="36">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="47"/>
@@ -2133,13 +2169,13 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>75</v>
       </c>
       <c r="C40" s="37">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D40" s="45"/>
       <c r="E40" s="47"/>
@@ -2150,15 +2186,15 @@
       <c r="L40" s="27"/>
       <c r="M40" s="27"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="37">
-        <v>20</v>
+    <row r="41" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="36">
+        <v>12</v>
       </c>
       <c r="D41" s="45"/>
       <c r="E41" s="47"/>
@@ -2170,11 +2206,11 @@
       <c r="M41" s="27"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
-        <v>82</v>
+      <c r="A42" s="20" t="s">
+        <v>78</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C42" s="37">
         <v>12</v>
@@ -2190,13 +2226,13 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C43" s="37">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D43" s="45"/>
       <c r="E43" s="47"/>
@@ -2207,15 +2243,15 @@
       <c r="L43" s="27"/>
       <c r="M43" s="27"/>
     </row>
-    <row r="44" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="36">
-        <v>24</v>
+        <v>82</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="37">
+        <v>12</v>
       </c>
       <c r="D44" s="45"/>
       <c r="E44" s="47"/>
@@ -2228,13 +2264,13 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C45" s="37">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D45" s="45"/>
       <c r="E45" s="47"/>
@@ -2247,13 +2283,13 @@
     </row>
     <row r="46" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C46" s="36">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="47"/>
@@ -2264,15 +2300,15 @@
       <c r="L46" s="27"/>
       <c r="M46" s="27"/>
     </row>
-    <row r="47" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" s="38">
-        <v>10</v>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="37">
+        <v>24</v>
       </c>
       <c r="D47" s="45"/>
       <c r="E47" s="47"/>
@@ -2283,15 +2319,15 @@
       <c r="L47" s="27"/>
       <c r="M47" s="27"/>
     </row>
-    <row r="48" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="38">
-        <v>9</v>
+    <row r="48" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="36">
+        <v>12</v>
       </c>
       <c r="D48" s="45"/>
       <c r="E48" s="47"/>
@@ -2304,13 +2340,13 @@
     </row>
     <row r="49" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B49" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="39">
-        <v>24</v>
+        <v>92</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="38">
+        <v>10</v>
       </c>
       <c r="D49" s="45"/>
       <c r="E49" s="47"/>
@@ -2321,15 +2357,15 @@
       <c r="L49" s="27"/>
       <c r="M49" s="27"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="28">
-        <v>20</v>
+    <row r="50" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A50" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="38">
+        <v>9</v>
       </c>
       <c r="D50" s="45"/>
       <c r="E50" s="47"/>
@@ -2340,15 +2376,15 @@
       <c r="L50" s="27"/>
       <c r="M50" s="27"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C51" s="28">
-        <v>9</v>
+    <row r="51" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A51" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="39">
+        <v>24</v>
       </c>
       <c r="D51" s="45"/>
       <c r="E51" s="47"/>
@@ -2361,13 +2397,13 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C52" s="28">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D52" s="45"/>
       <c r="E52" s="47"/>
@@ -2380,13 +2416,13 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C53" s="28">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D53" s="45"/>
       <c r="E53" s="47"/>
@@ -2399,13 +2435,13 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C54" s="28">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="47"/>
@@ -2418,10 +2454,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C55" s="28">
         <v>24</v>
@@ -2437,13 +2473,13 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C56" s="28">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D56" s="45"/>
       <c r="E56" s="47"/>
@@ -2456,13 +2492,13 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C57" s="28">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D57" s="45"/>
       <c r="E57" s="47"/>
@@ -2475,13 +2511,13 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C58" s="28">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="D58" s="45"/>
       <c r="E58" s="47"/>
@@ -2494,13 +2530,13 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C59" s="28">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D59" s="45"/>
       <c r="E59" s="47"/>
@@ -2513,13 +2549,13 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C60" s="28">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D60" s="45"/>
       <c r="E60" s="47"/>
@@ -2532,13 +2568,13 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C61" s="28">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D61" s="45"/>
       <c r="E61" s="47"/>
@@ -2551,13 +2587,13 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C62" s="28">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D62" s="45"/>
       <c r="E62" s="47"/>
@@ -2570,13 +2606,13 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C63" s="28">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D63" s="45"/>
       <c r="E63" s="47"/>
@@ -2589,10 +2625,10 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C64" s="28">
         <v>12</v>
@@ -2608,13 +2644,13 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C65" s="28">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D65" s="45"/>
       <c r="E65" s="47"/>
@@ -2627,13 +2663,13 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C66" s="28">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D66" s="45"/>
       <c r="E66" s="47"/>
@@ -2646,13 +2682,13 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C67" s="28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D67" s="45"/>
       <c r="E67" s="47"/>
@@ -2663,25 +2699,63 @@
       <c r="L67" s="27"/>
       <c r="M67" s="27"/>
     </row>
-    <row r="68" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C68" s="28">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="D68" s="45"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="50"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="48"/>
       <c r="G68" s="46"/>
       <c r="I68" s="27"/>
       <c r="J68" s="27"/>
       <c r="L68" s="27"/>
       <c r="M68" s="27"/>
     </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="28">
+        <v>10</v>
+      </c>
+      <c r="D69" s="45"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="48"/>
+      <c r="G69" s="46"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="27"/>
+      <c r="L69" s="27"/>
+      <c r="M69" s="27"/>
+    </row>
+    <row r="70" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" s="28">
+        <v>60</v>
+      </c>
+      <c r="D70" s="45"/>
+      <c r="E70" s="49"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="46"/>
+      <c r="I70" s="27"/>
+      <c r="J70" s="27"/>
+      <c r="L70" s="27"/>
+      <c r="M70" s="27"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>